<commit_message>
Changing the way the excel files has been reading
In the real server office is not installed, so i can't use the ole12. So
I changed for a new third party library called NPOI that helps me to
read the file, it is not the best but it's working for now.
</commit_message>
<xml_diff>
--- a/SolucionesARWebsite/SolucionesARWebsite2/Files/example.xlsx
+++ b/SolucionesARWebsite/SolucionesARWebsite2/Files/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="90" windowWidth="8115" windowHeight="5190"/>
+    <workbookView xWindow="600" yWindow="90" windowWidth="8115" windowHeight="5190" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="mihoja" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="15">
   <si>
     <t>Campaña</t>
   </si>
@@ -57,7 +57,10 @@
     <t>eeee</t>
   </si>
   <si>
-    <t>2-0376-0842</t>
+    <t>6-0374-0270</t>
+  </si>
+  <si>
+    <t>6-03740270</t>
   </si>
 </sst>
 </file>
@@ -65,18 +68,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="&quot;₡&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;₡&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -104,12 +99,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,24 +445,18 @@
       <c r="C2" s="1">
         <v>41385</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>10000</v>
       </c>
       <c r="E2">
         <v>50</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>1000</v>
       </c>
       <c r="G2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G8" s="2"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G14" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -479,10 +466,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,17 +507,17 @@
       <c r="C2" s="1">
         <v>41385</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>10000</v>
       </c>
       <c r="E2">
         <v>50</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>1000</v>
       </c>
-      <c r="G2">
-        <v>203760842</v>
+      <c r="G2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -543,17 +530,17 @@
       <c r="C3" s="1">
         <v>41385</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>5000</v>
       </c>
       <c r="E3">
         <v>50</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>500</v>
       </c>
-      <c r="G3">
-        <v>203760842</v>
+      <c r="G3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -566,17 +553,17 @@
       <c r="C4" s="1">
         <v>41385</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>6000</v>
       </c>
       <c r="E4">
         <v>50</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>600</v>
       </c>
-      <c r="G4">
-        <v>203760842</v>
+      <c r="G4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -589,17 +576,17 @@
       <c r="C5" s="1">
         <v>41385</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>2000</v>
       </c>
       <c r="E5">
         <v>50</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>200</v>
       </c>
-      <c r="G5">
-        <v>203760842</v>
+      <c r="G5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -612,27 +599,22 @@
       <c r="C6" s="1">
         <v>41385</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>8000</v>
       </c>
       <c r="E6">
         <v>50</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <v>8000</v>
       </c>
-      <c r="G6">
-        <v>203760842</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G12" s="2"/>
-    </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G18" s="4"/>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>